<commit_message>
Added RandomForest Feature Selection
</commit_message>
<xml_diff>
--- a/data/EEG/EEG_Shifted_Correlation_Matrix.xlsx
+++ b/data/EEG/EEG_Shifted_Correlation_Matrix.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>var1(t-1)</t>
   </si>
@@ -58,9 +58,6 @@
     <t>var14(t-1)</t>
   </si>
   <si>
-    <t>var15(t-1)</t>
-  </si>
-  <si>
     <t>var1(t)</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
   </si>
   <si>
     <t>var14(t)</t>
-  </si>
-  <si>
-    <t>var15(t)</t>
   </si>
 </sst>
 </file>
@@ -461,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE31"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:29">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,14 +546,8 @@
       <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31">
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,88 +555,88 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.7702779598303846</v>
+        <v>0.8157148239077143</v>
       </c>
       <c r="D2">
-        <v>0.801437784703939</v>
+        <v>0.8043038899376217</v>
       </c>
       <c r="E2">
-        <v>0.8191204386059361</v>
+        <v>0.8108728847521418</v>
       </c>
       <c r="F2">
-        <v>0.4687623150274925</v>
+        <v>0.4217566772359677</v>
       </c>
       <c r="G2">
-        <v>-0.07977868213105821</v>
+        <v>-0.171950748104927</v>
       </c>
       <c r="H2">
-        <v>0.3806463326323112</v>
+        <v>0.3516131090247847</v>
       </c>
       <c r="I2">
-        <v>0.2635059656054787</v>
+        <v>0.2158781155275934</v>
       </c>
       <c r="J2">
-        <v>0.346894419782721</v>
+        <v>0.3005146752206763</v>
       </c>
       <c r="K2">
-        <v>0.5949996908441775</v>
+        <v>0.5495518617528315</v>
       </c>
       <c r="L2">
-        <v>0.8294940068901203</v>
+        <v>0.8129483257770075</v>
       </c>
       <c r="M2">
-        <v>0.8231637759004217</v>
+        <v>0.8111417588888375</v>
       </c>
       <c r="N2">
-        <v>0.9355540294197618</v>
+        <v>0.9293784147806209</v>
       </c>
       <c r="O2">
-        <v>0.8387828611289709</v>
+        <v>0.8281440442142266</v>
+      </c>
+      <c r="P2">
+        <v>0.8038319589424036</v>
       </c>
       <c r="Q2">
-        <v>0.813977352254015</v>
+        <v>0.6068633322525723</v>
       </c>
       <c r="R2">
-        <v>0.5244703043530895</v>
+        <v>0.6918603086908143</v>
       </c>
       <c r="S2">
-        <v>0.6650772527458279</v>
+        <v>0.7728348479056302</v>
       </c>
       <c r="T2">
-        <v>0.7631736456252456</v>
+        <v>0.2878861269933049</v>
       </c>
       <c r="U2">
-        <v>0.3031296075575655</v>
+        <v>-0.2121928915181684</v>
       </c>
       <c r="V2">
-        <v>-0.179735012042285</v>
+        <v>0.3427605892453699</v>
       </c>
       <c r="W2">
-        <v>0.3602083924845833</v>
+        <v>0.3008101258340814</v>
       </c>
       <c r="X2">
-        <v>0.3208719671130565</v>
+        <v>0.3143112137969718</v>
       </c>
       <c r="Y2">
-        <v>0.3507758699896558</v>
+        <v>0.532985201385787</v>
       </c>
       <c r="Z2">
-        <v>0.569420461432085</v>
+        <v>0.680090238281893</v>
       </c>
       <c r="AA2">
-        <v>0.6939573807517601</v>
+        <v>0.6316541923828297</v>
       </c>
       <c r="AB2">
-        <v>0.631942348003848</v>
+        <v>0.7680199484382367</v>
       </c>
       <c r="AC2">
-        <v>0.7831479068152678</v>
-      </c>
-      <c r="AD2">
-        <v>0.5833359684144496</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31">
+        <v>0.5659989996976429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -656,85 +644,85 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.4265273038297726</v>
+        <v>0.422930565280088</v>
       </c>
       <c r="E3">
-        <v>0.4417873603389675</v>
+        <v>0.4474523436422672</v>
       </c>
       <c r="F3">
-        <v>0.1817153518537629</v>
+        <v>0.1620598197201565</v>
       </c>
       <c r="G3">
-        <v>0.02289901448497412</v>
+        <v>0.01510015190361084</v>
       </c>
       <c r="H3">
-        <v>0.1207473168892882</v>
+        <v>0.1126358587754349</v>
       </c>
       <c r="I3">
-        <v>0.1968580493293127</v>
+        <v>0.1933690034700503</v>
       </c>
       <c r="J3">
-        <v>0.3351744221406798</v>
+        <v>0.338004623866562</v>
       </c>
       <c r="K3">
-        <v>0.6359489951514805</v>
+        <v>0.6815464859692254</v>
       </c>
       <c r="L3">
-        <v>0.7562720152988628</v>
+        <v>0.7963104058094024</v>
       </c>
       <c r="M3">
-        <v>0.6062266551406286</v>
+        <v>0.6219573507419136</v>
       </c>
       <c r="N3">
-        <v>0.7628835386823494</v>
+        <v>0.8156475574143959</v>
       </c>
       <c r="O3">
-        <v>0.7329853383659358</v>
+        <v>0.7871253174521233</v>
+      </c>
+      <c r="P3">
+        <v>0.5934852041566551</v>
       </c>
       <c r="Q3">
-        <v>0.5649508041009601</v>
+        <v>0.6438192685610078</v>
       </c>
       <c r="R3">
-        <v>0.6174611105044985</v>
+        <v>0.289745070141585</v>
       </c>
       <c r="S3">
-        <v>0.2845379110264941</v>
+        <v>0.4234050634642471</v>
       </c>
       <c r="T3">
-        <v>0.4138771882430116</v>
+        <v>-0.02271058058662566</v>
       </c>
       <c r="U3">
-        <v>-0.03542628314856379</v>
+        <v>-0.008178966105131124</v>
       </c>
       <c r="V3">
-        <v>0.01566916401809424</v>
+        <v>0.01896871498884205</v>
       </c>
       <c r="W3">
-        <v>0.00183348886981787</v>
+        <v>0.2909283867349914</v>
       </c>
       <c r="X3">
-        <v>0.2777136898855114</v>
+        <v>0.353402166577147</v>
       </c>
       <c r="Y3">
-        <v>0.3125905722899217</v>
+        <v>0.5789561113793267</v>
       </c>
       <c r="Z3">
-        <v>0.5359338098322962</v>
+        <v>0.5905187401413579</v>
       </c>
       <c r="AA3">
-        <v>0.5648745294839975</v>
+        <v>0.3668207673233485</v>
       </c>
       <c r="AB3">
-        <v>0.3567530473907892</v>
+        <v>0.6049630495909035</v>
       </c>
       <c r="AC3">
-        <v>0.563405981947166</v>
-      </c>
-      <c r="AD3">
-        <v>0.3858993714080252</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31">
+        <v>0.4012646185276836</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -742,82 +730,82 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.9524808993546569</v>
+        <v>0.9532452470082411</v>
       </c>
       <c r="F4">
-        <v>0.5982012114683596</v>
+        <v>0.582943070658333</v>
       </c>
       <c r="G4">
-        <v>-0.1118317509230324</v>
+        <v>-0.1611567809696591</v>
       </c>
       <c r="H4">
-        <v>0.6764353968098932</v>
+        <v>0.6671324918466492</v>
       </c>
       <c r="I4">
-        <v>0.3439580471759082</v>
+        <v>0.3212406662790502</v>
       </c>
       <c r="J4">
-        <v>0.2930096261729668</v>
+        <v>0.2663083660813142</v>
       </c>
       <c r="K4">
-        <v>0.317629201449202</v>
+        <v>0.2870172437297561</v>
       </c>
       <c r="L4">
-        <v>0.6141487213672582</v>
+        <v>0.6028461286448914</v>
       </c>
       <c r="M4">
-        <v>0.8672002496331838</v>
+        <v>0.8670267783807273</v>
       </c>
       <c r="N4">
-        <v>0.7378634136167521</v>
+        <v>0.7395315769245084</v>
       </c>
       <c r="O4">
-        <v>0.6708603946435894</v>
+        <v>0.6704464218553099</v>
+      </c>
+      <c r="P4">
+        <v>0.7553805872345052</v>
       </c>
       <c r="Q4">
-        <v>0.7557258892080677</v>
+        <v>0.350613642705196</v>
       </c>
       <c r="R4">
-        <v>0.3153146686521974</v>
+        <v>0.9388626813301555</v>
       </c>
       <c r="S4">
-        <v>0.927375412936201</v>
+        <v>0.960598349222287</v>
       </c>
       <c r="T4">
-        <v>0.9559796049856084</v>
+        <v>0.5129661623857951</v>
       </c>
       <c r="U4">
-        <v>0.5102314263567551</v>
+        <v>-0.2084758337442963</v>
       </c>
       <c r="V4">
-        <v>-0.1833563637995853</v>
+        <v>0.588096608055056</v>
       </c>
       <c r="W4">
-        <v>0.5828524429723282</v>
+        <v>0.2610062939132559</v>
       </c>
       <c r="X4">
-        <v>0.2699419258103936</v>
+        <v>0.1988705388061064</v>
       </c>
       <c r="Y4">
-        <v>0.2086060854245799</v>
+        <v>0.3009229925236416</v>
       </c>
       <c r="Z4">
-        <v>0.3194644123026967</v>
+        <v>0.5484908172447693</v>
       </c>
       <c r="AA4">
-        <v>0.5558117873529351</v>
+        <v>0.765525670881411</v>
       </c>
       <c r="AB4">
-        <v>0.7648350819803623</v>
+        <v>0.663762032764025</v>
       </c>
       <c r="AC4">
-        <v>0.663102443093212</v>
-      </c>
-      <c r="AD4">
-        <v>0.593736544463994</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31">
+        <v>0.5875005242921898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -825,79 +813,79 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.4941382783397901</v>
+        <v>0.4590491426498071</v>
       </c>
       <c r="G5">
-        <v>-0.2054170962865639</v>
+        <v>-0.280188908138834</v>
       </c>
       <c r="H5">
-        <v>0.5745040057222391</v>
+        <v>0.55797259424934</v>
       </c>
       <c r="I5">
-        <v>0.3151725067958286</v>
+        <v>0.2812810339864957</v>
       </c>
       <c r="J5">
-        <v>0.3067479568675213</v>
+        <v>0.2691469227936752</v>
       </c>
       <c r="K5">
-        <v>0.3871708951498321</v>
+        <v>0.3415348903779455</v>
       </c>
       <c r="L5">
-        <v>0.6162504783489366</v>
+        <v>0.5908312723483961</v>
       </c>
       <c r="M5">
-        <v>0.798240398410503</v>
+        <v>0.7864394106427642</v>
       </c>
       <c r="N5">
-        <v>0.7354988405394635</v>
+        <v>0.7210990987635891</v>
       </c>
       <c r="O5">
-        <v>0.6522588359739281</v>
+        <v>0.6310319453679272</v>
+      </c>
+      <c r="P5">
+        <v>0.6883138601789847</v>
       </c>
       <c r="Q5">
-        <v>0.7000682509992583</v>
+        <v>0.2862755348560969</v>
       </c>
       <c r="R5">
-        <v>0.2399925329646493</v>
+        <v>0.8517717936299758</v>
       </c>
       <c r="S5">
-        <v>0.8337233480207515</v>
+        <v>0.9190979316964288</v>
       </c>
       <c r="T5">
-        <v>0.9123533264942686</v>
+        <v>0.4274124369624318</v>
       </c>
       <c r="U5">
-        <v>0.4312010259362114</v>
+        <v>-0.3125996436185174</v>
       </c>
       <c r="V5">
-        <v>-0.2804304895761676</v>
+        <v>0.4285594253013059</v>
       </c>
       <c r="W5">
-        <v>0.4342409479505307</v>
+        <v>0.2272141609522264</v>
       </c>
       <c r="X5">
-        <v>0.2436935601244819</v>
+        <v>0.2117948120155193</v>
       </c>
       <c r="Y5">
-        <v>0.2361135340416304</v>
+        <v>0.3229957999351678</v>
       </c>
       <c r="Z5">
-        <v>0.3572092447501755</v>
+        <v>0.4092380449518906</v>
       </c>
       <c r="AA5">
-        <v>0.4308565188659603</v>
+        <v>0.6147657006240832</v>
       </c>
       <c r="AB5">
-        <v>0.6185001332422281</v>
+        <v>0.5685245608829964</v>
       </c>
       <c r="AC5">
-        <v>0.5859895283299082</v>
-      </c>
-      <c r="AD5">
-        <v>0.4665177496949859</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31">
+        <v>0.4486720923765558</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -905,76 +893,76 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.109285233820757</v>
+        <v>0.03032648073780352</v>
       </c>
       <c r="H6">
-        <v>0.419795128984058</v>
+        <v>0.3902983509787438</v>
       </c>
       <c r="I6">
-        <v>0.1546394956406064</v>
+        <v>0.0938639163677169</v>
       </c>
       <c r="J6">
-        <v>0.3309075192348947</v>
+        <v>0.2796410798167632</v>
       </c>
       <c r="K6">
-        <v>0.3994614136185505</v>
+        <v>0.3347151386100082</v>
       </c>
       <c r="L6">
-        <v>0.5379583454764266</v>
+        <v>0.4908791030292238</v>
       </c>
       <c r="M6">
-        <v>0.635575824222955</v>
+        <v>0.601466181700454</v>
       </c>
       <c r="N6">
-        <v>0.5535836259154702</v>
+        <v>0.5072937541697077</v>
       </c>
       <c r="O6">
-        <v>0.5973949518057131</v>
+        <v>0.5390032444114482</v>
+      </c>
+      <c r="P6">
+        <v>0.4957351293082953</v>
       </c>
       <c r="Q6">
-        <v>0.5168150893392084</v>
+        <v>0.2191058898951088</v>
       </c>
       <c r="R6">
-        <v>0.1533112223578368</v>
+        <v>0.5381760830210324</v>
       </c>
       <c r="S6">
-        <v>0.5121896378145039</v>
+        <v>0.5335839650369355</v>
       </c>
       <c r="T6">
-        <v>0.5286103587387381</v>
+        <v>0.5720313918734747</v>
       </c>
       <c r="U6">
-        <v>0.5539462827587381</v>
+        <v>0.1755352089074564</v>
       </c>
       <c r="V6">
-        <v>0.2024117287578417</v>
+        <v>0.3039533416234838</v>
       </c>
       <c r="W6">
-        <v>0.305649795966995</v>
+        <v>0.05461996064404375</v>
       </c>
       <c r="X6">
-        <v>0.08097979882472649</v>
+        <v>-0.03719091535177802</v>
       </c>
       <c r="Y6">
-        <v>0.004954514044532441</v>
+        <v>0.1707878834410803</v>
       </c>
       <c r="Z6">
-        <v>0.2249814872297362</v>
+        <v>0.4687883767699024</v>
       </c>
       <c r="AA6">
-        <v>0.4853483115101726</v>
+        <v>0.4884240553378977</v>
       </c>
       <c r="AB6">
-        <v>0.4881070170212619</v>
+        <v>0.5354984183694655</v>
       </c>
       <c r="AC6">
-        <v>0.5529628339740279</v>
-      </c>
-      <c r="AD6">
-        <v>0.5694726192834052</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31">
+        <v>0.5621766639964069</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -982,73 +970,73 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.1068960876843426</v>
+        <v>0.06474666132004668</v>
       </c>
       <c r="I7">
-        <v>0.2057008059025632</v>
+        <v>0.1590906736433282</v>
       </c>
       <c r="J7">
-        <v>0.1453000369112251</v>
+        <v>0.08999010760077723</v>
       </c>
       <c r="K7">
-        <v>0.1611204149560727</v>
+        <v>0.07822615126584806</v>
       </c>
       <c r="L7">
-        <v>0.1478366919264009</v>
+        <v>0.07163111762359774</v>
       </c>
       <c r="M7">
-        <v>0.1456562897747685</v>
+        <v>0.08007486022329285</v>
       </c>
       <c r="N7">
-        <v>0.08222259220071124</v>
+        <v>-0.00799374005574543</v>
       </c>
       <c r="O7">
-        <v>0.21139122550146</v>
+        <v>0.1196781618382669</v>
+      </c>
+      <c r="P7">
+        <v>0.02878804078666281</v>
       </c>
       <c r="Q7">
-        <v>0.08508059408060055</v>
+        <v>0.1572535815557266</v>
       </c>
       <c r="R7">
-        <v>0.1074826998825565</v>
+        <v>-0.03661316340294699</v>
       </c>
       <c r="S7">
-        <v>-0.03111329007442525</v>
+        <v>-0.07689685174881584</v>
       </c>
       <c r="T7">
-        <v>-0.04838421590155638</v>
+        <v>-0.1354343282638838</v>
       </c>
       <c r="U7">
-        <v>-0.1042434020240373</v>
+        <v>0.56938472093625</v>
       </c>
       <c r="V7">
-        <v>0.5647862909727296</v>
+        <v>0.1383039014186286</v>
       </c>
       <c r="W7">
-        <v>0.1622552888891805</v>
+        <v>0.1428508143238854</v>
       </c>
       <c r="X7">
-        <v>0.1675239513230579</v>
+        <v>0.2492234892517641</v>
       </c>
       <c r="Y7">
-        <v>0.2825469591721789</v>
+        <v>0.05611525031613714</v>
       </c>
       <c r="Z7">
-        <v>0.1222237525055679</v>
+        <v>0.2249295460667556</v>
       </c>
       <c r="AA7">
-        <v>0.2625477390275373</v>
+        <v>0.07912762461736503</v>
       </c>
       <c r="AB7">
-        <v>0.104365539311853</v>
+        <v>0.1592329895560755</v>
       </c>
       <c r="AC7">
-        <v>0.2142436111751265</v>
-      </c>
-      <c r="AD7">
-        <v>0.1674074094502347</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31">
+        <v>0.12922049944721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1056,70 +1044,70 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.4328517543750014</v>
+        <v>0.4113544396724342</v>
       </c>
       <c r="J8">
-        <v>0.25024868460154</v>
+        <v>0.2190322363369195</v>
       </c>
       <c r="K8">
-        <v>0.1845953233215067</v>
+        <v>0.1369673991367907</v>
       </c>
       <c r="L8">
-        <v>0.4478744623683059</v>
+        <v>0.4210536041441179</v>
       </c>
       <c r="M8">
-        <v>0.6282163634175637</v>
+        <v>0.6127537371377021</v>
       </c>
       <c r="N8">
-        <v>0.4105811899516785</v>
+        <v>0.380872270374958</v>
       </c>
       <c r="O8">
-        <v>0.4919372107544949</v>
+        <v>0.4677536622483949</v>
+      </c>
+      <c r="P8">
+        <v>0.4384699125292263</v>
       </c>
       <c r="Q8">
-        <v>0.4562593541836766</v>
+        <v>0.2050188016377254</v>
       </c>
       <c r="R8">
-        <v>0.1713583608032881</v>
+        <v>0.745010557723763</v>
       </c>
       <c r="S8">
-        <v>0.7359662500142738</v>
+        <v>0.7330213776490444</v>
       </c>
       <c r="T8">
-        <v>0.7340988118772703</v>
+        <v>0.3746249577488504</v>
       </c>
       <c r="U8">
-        <v>0.3789639451806685</v>
+        <v>-0.0646659550801988</v>
       </c>
       <c r="V8">
-        <v>-0.04533026395855345</v>
+        <v>0.7373554859336839</v>
       </c>
       <c r="W8">
-        <v>0.732524699341575</v>
+        <v>0.3844454745826349</v>
       </c>
       <c r="X8">
-        <v>0.3936427503616811</v>
+        <v>0.3100440472545577</v>
       </c>
       <c r="Y8">
-        <v>0.3223494234459123</v>
+        <v>0.2536504173312565</v>
       </c>
       <c r="Z8">
-        <v>0.2817578827571066</v>
+        <v>0.4280499070356468</v>
       </c>
       <c r="AA8">
-        <v>0.4436761400271373</v>
+        <v>0.6252441658377029</v>
       </c>
       <c r="AB8">
-        <v>0.6293379598347751</v>
+        <v>0.4487598273669594</v>
       </c>
       <c r="AC8">
-        <v>0.4654222010930836</v>
-      </c>
-      <c r="AD8">
-        <v>0.5186469108120387</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31">
+        <v>0.5065639187334045</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1127,67 +1115,67 @@
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0.7909851632684858</v>
+        <v>0.7803194042859418</v>
       </c>
       <c r="K9">
-        <v>0.4976929568416217</v>
+        <v>0.4641842567409938</v>
       </c>
       <c r="L9">
-        <v>0.3361846675522683</v>
+        <v>0.2909515270499535</v>
       </c>
       <c r="M9">
-        <v>0.3877151099700887</v>
+        <v>0.3506303276683601</v>
       </c>
       <c r="N9">
-        <v>0.2648861305205295</v>
+        <v>0.2106578977862553</v>
       </c>
       <c r="O9">
-        <v>0.2857132265386139</v>
+        <v>0.2232830090390359</v>
+      </c>
+      <c r="P9">
+        <v>0.02940061890293926</v>
       </c>
       <c r="Q9">
-        <v>0.07304175441544174</v>
+        <v>-0.04264217569197237</v>
       </c>
       <c r="R9">
-        <v>-0.07515422271669615</v>
+        <v>0.2642042121419276</v>
       </c>
       <c r="S9">
-        <v>0.2613949467895908</v>
+        <v>0.2703473767377377</v>
       </c>
       <c r="T9">
-        <v>0.2827825917350821</v>
+        <v>-0.2271624283349396</v>
       </c>
       <c r="U9">
-        <v>-0.2019920316448062</v>
+        <v>0.1877461119817939</v>
       </c>
       <c r="V9">
-        <v>0.2012375527804637</v>
+        <v>0.3983078447741007</v>
       </c>
       <c r="W9">
-        <v>0.4059374380329386</v>
+        <v>0.7657420463703245</v>
       </c>
       <c r="X9">
-        <v>0.7654820555423021</v>
+        <v>0.2873675688682911</v>
       </c>
       <c r="Y9">
-        <v>0.307814079820803</v>
+        <v>0.1366649037187454</v>
       </c>
       <c r="Z9">
-        <v>0.1818827071512769</v>
+        <v>-0.03268017545138932</v>
       </c>
       <c r="AA9">
-        <v>0.007221010405018141</v>
+        <v>0.1453618304914655</v>
       </c>
       <c r="AB9">
-        <v>0.1633020992477049</v>
+        <v>-0.03612480241228415</v>
       </c>
       <c r="AC9">
-        <v>0.01676111515665008</v>
-      </c>
-      <c r="AD9">
-        <v>0.086913329874987</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31">
+        <v>0.05426807656648059</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1195,64 +1183,64 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.7111129939900501</v>
+        <v>0.6926240927566955</v>
       </c>
       <c r="L10">
-        <v>0.5335399363856628</v>
+        <v>0.4992449856932368</v>
       </c>
       <c r="M10">
-        <v>0.4199695264570207</v>
+        <v>0.3810484361532144</v>
       </c>
       <c r="N10">
-        <v>0.421489221654538</v>
+        <v>0.3755964262284131</v>
       </c>
       <c r="O10">
-        <v>0.3766718780310199</v>
+        <v>0.3178935776891257</v>
+      </c>
+      <c r="P10">
+        <v>0.2117181168144797</v>
       </c>
       <c r="Q10">
-        <v>0.2498126279754389</v>
+        <v>0.2295228886268328</v>
       </c>
       <c r="R10">
-        <v>0.1832519900533938</v>
+        <v>0.1868484903480842</v>
       </c>
       <c r="S10">
-        <v>0.1852931638506876</v>
+        <v>0.232733227071864</v>
       </c>
       <c r="T10">
-        <v>0.2470208427019577</v>
+        <v>0.02425585624744044</v>
       </c>
       <c r="U10">
-        <v>0.04317308769027269</v>
+        <v>0.2668992885214212</v>
       </c>
       <c r="V10">
-        <v>0.2783375906213771</v>
+        <v>0.08584403960841741</v>
       </c>
       <c r="W10">
-        <v>0.1063385828345069</v>
+        <v>0.7844870571688496</v>
       </c>
       <c r="X10">
-        <v>0.7824088915200423</v>
+        <v>0.5106307141722658</v>
       </c>
       <c r="Y10">
-        <v>0.5202783816150813</v>
+        <v>0.5376645951716087</v>
       </c>
       <c r="Z10">
-        <v>0.5602499676823197</v>
+        <v>0.1779064175750045</v>
       </c>
       <c r="AA10">
-        <v>0.2117681655523432</v>
+        <v>0.1852546915979612</v>
       </c>
       <c r="AB10">
-        <v>0.2032821334397607</v>
+        <v>0.1543629143761998</v>
       </c>
       <c r="AC10">
-        <v>0.2001141898268375</v>
-      </c>
-      <c r="AD10">
-        <v>0.3151151306185743</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31">
+        <v>0.2894175914966318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1260,61 +1248,61 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.7189981911182877</v>
+        <v>0.686634597145828</v>
       </c>
       <c r="M11">
-        <v>0.4936599831248249</v>
+        <v>0.4458359604219055</v>
       </c>
       <c r="N11">
-        <v>0.662324103764081</v>
+        <v>0.6180215299656138</v>
       </c>
       <c r="O11">
-        <v>0.7144765423141514</v>
+        <v>0.6754968759869173</v>
+      </c>
+      <c r="P11">
+        <v>0.3414106246871842</v>
       </c>
       <c r="Q11">
-        <v>0.3888982204227698</v>
+        <v>0.4263447240697736</v>
       </c>
       <c r="R11">
-        <v>0.3409989410854294</v>
+        <v>0.1786096219901734</v>
       </c>
       <c r="S11">
-        <v>0.1733082167528131</v>
+        <v>0.3079926957485415</v>
       </c>
       <c r="T11">
-        <v>0.321327944569617</v>
+        <v>-0.006674928344853386</v>
       </c>
       <c r="U11">
-        <v>0.02872148943754852</v>
+        <v>0.2423436613732328</v>
       </c>
       <c r="V11">
-        <v>0.2497931667089398</v>
+        <v>-0.09311803156270911</v>
       </c>
       <c r="W11">
-        <v>-0.04390791464069514</v>
+        <v>0.4750021626015974</v>
       </c>
       <c r="X11">
-        <v>0.4838544789344844</v>
+        <v>0.375027361438931</v>
       </c>
       <c r="Y11">
-        <v>0.4097106432758318</v>
+        <v>0.5948046322549021</v>
       </c>
       <c r="Z11">
-        <v>0.6292061515804794</v>
+        <v>0.3284890007893782</v>
       </c>
       <c r="AA11">
-        <v>0.3684949947029257</v>
+        <v>0.2106518013184411</v>
       </c>
       <c r="AB11">
-        <v>0.2342762663124268</v>
+        <v>0.4057833389203602</v>
       </c>
       <c r="AC11">
-        <v>0.4554066539837696</v>
-      </c>
-      <c r="AD11">
-        <v>0.3599841315967257</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31">
+        <v>0.3254607882489869</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1322,58 +1310,58 @@
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0.8302022208341028</v>
+        <v>0.8160014486515024</v>
       </c>
       <c r="N12">
-        <v>0.9261555814250847</v>
+        <v>0.9182562569080269</v>
       </c>
       <c r="O12">
-        <v>0.8837994759679769</v>
+        <v>0.8738417930415344</v>
+      </c>
+      <c r="P12">
+        <v>0.68944687124684</v>
       </c>
       <c r="Q12">
-        <v>0.7056887589095076</v>
+        <v>0.6386552242537881</v>
       </c>
       <c r="R12">
-        <v>0.5491279705782476</v>
+        <v>0.4871942566841443</v>
       </c>
       <c r="S12">
-        <v>0.4677847194343153</v>
+        <v>0.6394167568132799</v>
       </c>
       <c r="T12">
-        <v>0.6343890718828091</v>
+        <v>0.1735971237094873</v>
       </c>
       <c r="U12">
-        <v>0.1920901272477452</v>
+        <v>-0.01289574416276831</v>
       </c>
       <c r="V12">
-        <v>0.01425580662621996</v>
+        <v>0.2049187045249005</v>
       </c>
       <c r="W12">
-        <v>0.2267778389722594</v>
+        <v>0.4461323864028962</v>
       </c>
       <c r="X12">
-        <v>0.4561196924938045</v>
+        <v>0.5095600740822565</v>
       </c>
       <c r="Y12">
-        <v>0.5253434653954384</v>
+        <v>0.6730393216477163</v>
       </c>
       <c r="Z12">
-        <v>0.694650126256277</v>
+        <v>0.7228082890689547</v>
       </c>
       <c r="AA12">
-        <v>0.7313772547550319</v>
+        <v>0.5064038707059239</v>
       </c>
       <c r="AB12">
-        <v>0.5114536040594347</v>
+        <v>0.7092893076849008</v>
       </c>
       <c r="AC12">
-        <v>0.7260479670846383</v>
-      </c>
-      <c r="AD12">
-        <v>0.6118336386141587</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31">
+        <v>0.5982566943196098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1381,55 +1369,55 @@
         <v>1</v>
       </c>
       <c r="N13">
-        <v>0.835730260339285</v>
+        <v>0.8236578926619049</v>
       </c>
       <c r="O13">
-        <v>0.841021362262341</v>
+        <v>0.8301993558007128</v>
+      </c>
+      <c r="P13">
+        <v>0.7214580737500552</v>
       </c>
       <c r="Q13">
-        <v>0.7317116685383522</v>
+        <v>0.489828314179937</v>
       </c>
       <c r="R13">
-        <v>0.4208973839618185</v>
+        <v>0.7687770496407018</v>
       </c>
       <c r="S13">
-        <v>0.7429321064367033</v>
+        <v>0.8388783440535271</v>
       </c>
       <c r="T13">
-        <v>0.8274604684100469</v>
+        <v>0.4317177798437138</v>
       </c>
       <c r="U13">
-        <v>0.4323019729278197</v>
+        <v>0.009718598397346827</v>
       </c>
       <c r="V13">
-        <v>0.0371517811394295</v>
+        <v>0.5382495460842696</v>
       </c>
       <c r="W13">
-        <v>0.5358519341372034</v>
+        <v>0.403284668302877</v>
       </c>
       <c r="X13">
-        <v>0.4131597017157597</v>
+        <v>0.3963753156646265</v>
       </c>
       <c r="Y13">
-        <v>0.4109612323353216</v>
+        <v>0.4713775699286663</v>
       </c>
       <c r="Z13">
-        <v>0.5009102692988032</v>
+        <v>0.7273430364741758</v>
       </c>
       <c r="AA13">
-        <v>0.7333793871532008</v>
+        <v>0.759749059991311</v>
       </c>
       <c r="AB13">
-        <v>0.7534128601718668</v>
+        <v>0.7080554878031393</v>
       </c>
       <c r="AC13">
-        <v>0.7181881196892584</v>
-      </c>
-      <c r="AD13">
-        <v>0.6537052596381395</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31">
+        <v>0.6448739384993679</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1437,107 +1425,149 @@
         <v>1</v>
       </c>
       <c r="O14">
-        <v>0.885104322125238</v>
+        <v>0.8735937662682089</v>
+      </c>
+      <c r="P14">
+        <v>0.8238642315684102</v>
       </c>
       <c r="Q14">
-        <v>0.8300289256885708</v>
+        <v>0.6592108853650348</v>
       </c>
       <c r="R14">
-        <v>0.558108653227459</v>
+        <v>0.6526095339397402</v>
       </c>
       <c r="S14">
-        <v>0.6193031421763656</v>
+        <v>0.7465090906525405</v>
       </c>
       <c r="T14">
-        <v>0.7317660997685141</v>
+        <v>0.2901856598434125</v>
       </c>
       <c r="U14">
-        <v>0.3041955692796396</v>
+        <v>-0.1027402830892206</v>
       </c>
       <c r="V14">
-        <v>-0.07013735997594348</v>
+        <v>0.2124496997257917</v>
       </c>
       <c r="W14">
-        <v>0.2379930152062062</v>
+        <v>0.3622150623992543</v>
       </c>
       <c r="X14">
-        <v>0.3782604398458148</v>
+        <v>0.4358617045729148</v>
       </c>
       <c r="Y14">
-        <v>0.4630696216017583</v>
+        <v>0.5765650987491241</v>
       </c>
       <c r="Z14">
-        <v>0.6115197538946013</v>
+        <v>0.7505751828589649</v>
       </c>
       <c r="AA14">
-        <v>0.7569658731538651</v>
+        <v>0.6334212067969673</v>
       </c>
       <c r="AB14">
-        <v>0.6291398892012539</v>
+        <v>0.8198950364539799</v>
       </c>
       <c r="AC14">
-        <v>0.8292424024513805</v>
-      </c>
-      <c r="AD14">
-        <v>0.6216928111675882</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31">
+        <v>0.6086501002796603</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
+      <c r="P15">
+        <v>0.753337583534509</v>
+      </c>
       <c r="Q15">
-        <v>0.7534726335143218</v>
+        <v>0.6919132780056105</v>
       </c>
       <c r="R15">
-        <v>0.55825177526867</v>
+        <v>0.5948607862901633</v>
       </c>
       <c r="S15">
-        <v>0.5488891546470059</v>
+        <v>0.693252933919704</v>
       </c>
       <c r="T15">
-        <v>0.6668549483177821</v>
+        <v>0.2319352912410659</v>
       </c>
       <c r="U15">
-        <v>0.2412969736913865</v>
+        <v>0.08235996380124101</v>
       </c>
       <c r="V15">
-        <v>0.1153766421951369</v>
+        <v>0.2946403570534328</v>
       </c>
       <c r="W15">
-        <v>0.3033444829771899</v>
+        <v>0.2507280716924482</v>
       </c>
       <c r="X15">
-        <v>0.2698106195093072</v>
+        <v>0.2703657291944395</v>
       </c>
       <c r="Y15">
-        <v>0.3020780159824433</v>
+        <v>0.5456486381248949</v>
       </c>
       <c r="Z15">
-        <v>0.5766271735530039</v>
+        <v>0.7196196970636767</v>
       </c>
       <c r="AA15">
-        <v>0.715330767759627</v>
+        <v>0.6247781202214415</v>
       </c>
       <c r="AB15">
-        <v>0.6078728788439243</v>
+        <v>0.7988404738082945</v>
       </c>
       <c r="AC15">
-        <v>0.795654570356861</v>
-      </c>
-      <c r="AD15">
-        <v>0.6517534907894331</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31">
+        <v>0.6534095979737364</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:30">
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>0.8206062678165131</v>
+      </c>
+      <c r="R16">
+        <v>0.7964502078226058</v>
+      </c>
+      <c r="S16">
+        <v>0.8109301582428132</v>
+      </c>
+      <c r="T16">
+        <v>0.4155038327026787</v>
+      </c>
+      <c r="U16">
+        <v>-0.1346558024751652</v>
+      </c>
+      <c r="V16">
+        <v>0.3236025664916114</v>
+      </c>
+      <c r="W16">
+        <v>0.1760547658865114</v>
+      </c>
+      <c r="X16">
+        <v>0.2905733560716632</v>
+      </c>
+      <c r="Y16">
+        <v>0.5613648020883134</v>
+      </c>
+      <c r="Z16">
+        <v>0.8193955358415558</v>
+      </c>
+      <c r="AA16">
+        <v>0.8146652778365542</v>
+      </c>
+      <c r="AB16">
+        <v>0.9295315771563073</v>
+      </c>
+      <c r="AC16">
+        <v>0.8275976929379294</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1545,46 +1575,43 @@
         <v>1</v>
       </c>
       <c r="R17">
-        <v>0.7543278936121034</v>
+        <v>0.4273060493414992</v>
       </c>
       <c r="S17">
-        <v>0.7792692337635851</v>
+        <v>0.4523880366474143</v>
       </c>
       <c r="T17">
-        <v>0.8081787003853479</v>
+        <v>0.170229695903207</v>
       </c>
       <c r="U17">
-        <v>0.4273052625816671</v>
+        <v>0.03315134890435142</v>
       </c>
       <c r="V17">
-        <v>-0.1188940037625209</v>
+        <v>0.107257328427798</v>
       </c>
       <c r="W17">
-        <v>0.3429026884218027</v>
+        <v>0.1928284544485881</v>
       </c>
       <c r="X17">
-        <v>0.198791356188484</v>
+        <v>0.3432537001654004</v>
       </c>
       <c r="Y17">
-        <v>0.3248398670043175</v>
+        <v>0.6803622914595607</v>
       </c>
       <c r="Z17">
-        <v>0.5883536196417281</v>
+        <v>0.7923434539905985</v>
       </c>
       <c r="AA17">
-        <v>0.8270679697315511</v>
+        <v>0.6245570216718043</v>
       </c>
       <c r="AB17">
-        <v>0.8137689923151294</v>
+        <v>0.8142806494171361</v>
       </c>
       <c r="AC17">
-        <v>0.9325722311102529</v>
-      </c>
-      <c r="AD17">
-        <v>0.833267041690548</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30">
+        <v>0.7670170028272626</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1592,43 +1619,40 @@
         <v>1</v>
       </c>
       <c r="S18">
-        <v>0.4192298192790167</v>
+        <v>0.9532854241619281</v>
       </c>
       <c r="T18">
-        <v>0.4291991379264885</v>
+        <v>0.5565277553921529</v>
       </c>
       <c r="U18">
-        <v>0.1522827238775791</v>
+        <v>-0.1493354467743147</v>
       </c>
       <c r="V18">
-        <v>0.0183292054962371</v>
+        <v>0.6469956337958054</v>
       </c>
       <c r="W18">
-        <v>0.08719139504302025</v>
+        <v>0.2696796266081678</v>
       </c>
       <c r="X18">
-        <v>0.1706437010545848</v>
+        <v>0.2379407626144594</v>
       </c>
       <c r="Y18">
-        <v>0.299649924910132</v>
+        <v>0.2831100992051486</v>
       </c>
       <c r="Z18">
-        <v>0.6022776027588421</v>
+        <v>0.6005558988921768</v>
       </c>
       <c r="AA18">
-        <v>0.737173279905999</v>
+        <v>0.8628582518407122</v>
       </c>
       <c r="AB18">
-        <v>0.5956709926923578</v>
+        <v>0.7295764383808694</v>
       </c>
       <c r="AC18">
-        <v>0.7350138385626431</v>
-      </c>
-      <c r="AD18">
-        <v>0.718860627496073</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30">
+        <v>0.6563180053807268</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1636,40 +1660,37 @@
         <v>1</v>
       </c>
       <c r="T19">
-        <v>0.9501647718840887</v>
+        <v>0.4567082044727581</v>
       </c>
       <c r="U19">
-        <v>0.5534951538115263</v>
+        <v>-0.2465614110513088</v>
       </c>
       <c r="V19">
-        <v>-0.1470322778453364</v>
+        <v>0.5462385753544525</v>
       </c>
       <c r="W19">
-        <v>0.6407270801048023</v>
+        <v>0.2548086742838339</v>
       </c>
       <c r="X19">
-        <v>0.269482364773024</v>
+        <v>0.2610310340043945</v>
       </c>
       <c r="Y19">
-        <v>0.2339946698245965</v>
+        <v>0.353960827575866</v>
       </c>
       <c r="Z19">
-        <v>0.2759961127082147</v>
+        <v>0.5981092747210899</v>
       </c>
       <c r="AA19">
-        <v>0.5919139765368145</v>
+        <v>0.7877341511334522</v>
       </c>
       <c r="AB19">
-        <v>0.8591851495610711</v>
+        <v>0.7219859656781238</v>
       </c>
       <c r="AC19">
-        <v>0.7069597285845243</v>
-      </c>
-      <c r="AD19">
-        <v>0.6489899641917518</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30">
+        <v>0.6336582151877339</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1677,37 +1698,34 @@
         <v>1</v>
       </c>
       <c r="U20">
-        <v>0.4614649941430777</v>
+        <v>0.06878708871226616</v>
       </c>
       <c r="V20">
-        <v>-0.2374281495967844</v>
+        <v>0.3327386784654857</v>
       </c>
       <c r="W20">
-        <v>0.5497620644018684</v>
+        <v>-0.004237113518879295</v>
       </c>
       <c r="X20">
-        <v>0.2637483159411842</v>
+        <v>0.2509890592050743</v>
       </c>
       <c r="Y20">
-        <v>0.2727786441824856</v>
+        <v>0.3559606344080504</v>
       </c>
       <c r="Z20">
-        <v>0.3652206031325668</v>
+        <v>0.5150822877451552</v>
       </c>
       <c r="AA20">
-        <v>0.6027901002681968</v>
+        <v>0.6148761538787972</v>
       </c>
       <c r="AB20">
-        <v>0.7899668612111165</v>
+        <v>0.5162774163167224</v>
       </c>
       <c r="AC20">
-        <v>0.7180121524301792</v>
-      </c>
-      <c r="AD20">
-        <v>0.638012758002795</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30">
+        <v>0.5728582987705447</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1715,34 +1733,31 @@
         <v>1</v>
       </c>
       <c r="V21">
-        <v>0.06460933223953363</v>
+        <v>0.07105770371787114</v>
       </c>
       <c r="W21">
-        <v>0.3467795952593964</v>
+        <v>0.1710954601543539</v>
       </c>
       <c r="X21">
-        <v>0.01186636971191807</v>
+        <v>0.1119301267207387</v>
       </c>
       <c r="Y21">
-        <v>0.2738506818697914</v>
+        <v>0.1229410565812919</v>
       </c>
       <c r="Z21">
-        <v>0.3728465510115321</v>
+        <v>0.1155618732212763</v>
       </c>
       <c r="AA21">
-        <v>0.5237794782005266</v>
+        <v>0.1178261198574178</v>
       </c>
       <c r="AB21">
-        <v>0.6185767698622812</v>
+        <v>0.03725586859447715</v>
       </c>
       <c r="AC21">
-        <v>0.5256647194198487</v>
-      </c>
-      <c r="AD21">
-        <v>0.5792782663704971</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30">
+        <v>0.1810950226532188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1750,31 +1765,28 @@
         <v>1</v>
       </c>
       <c r="W22">
-        <v>0.06562764155190491</v>
+        <v>0.3475807097910168</v>
       </c>
       <c r="X22">
-        <v>0.1711072601593547</v>
+        <v>0.1744235451201039</v>
       </c>
       <c r="Y22">
-        <v>0.1031952773168788</v>
+        <v>0.1227868929670771</v>
       </c>
       <c r="Z22">
-        <v>0.1262417835747769</v>
+        <v>0.4152173184443029</v>
       </c>
       <c r="AA22">
-        <v>0.1206256393557973</v>
+        <v>0.6046384577942131</v>
       </c>
       <c r="AB22">
-        <v>0.1212929396511327</v>
+        <v>0.3599322991845473</v>
       </c>
       <c r="AC22">
-        <v>0.04437190516645813</v>
-      </c>
-      <c r="AD22">
-        <v>0.1849421592586445</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30">
+        <v>0.4562718795903771</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1782,28 +1794,25 @@
         <v>1</v>
       </c>
       <c r="X23">
-        <v>0.3597425150080412</v>
+        <v>0.7720401239632422</v>
       </c>
       <c r="Y23">
-        <v>0.2070480619444518</v>
+        <v>0.4611022074012511</v>
       </c>
       <c r="Z23">
-        <v>0.1583622604885944</v>
+        <v>0.2848433131222219</v>
       </c>
       <c r="AA23">
-        <v>0.4300127813115558</v>
+        <v>0.3356669851495188</v>
       </c>
       <c r="AB23">
-        <v>0.6086505748461924</v>
+        <v>0.1815545509943996</v>
       </c>
       <c r="AC23">
-        <v>0.3820744544060634</v>
-      </c>
-      <c r="AD23">
-        <v>0.4679043835606026</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30">
+        <v>0.2187172174946918</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1811,25 +1820,22 @@
         <v>1</v>
       </c>
       <c r="Y24">
-        <v>0.7720915637779822</v>
+        <v>0.6955789831032103</v>
       </c>
       <c r="Z24">
-        <v>0.4748842135457912</v>
+        <v>0.5060210135431616</v>
       </c>
       <c r="AA24">
-        <v>0.3020636228886074</v>
+        <v>0.3817519343868738</v>
       </c>
       <c r="AB24">
-        <v>0.3449334770647883</v>
+        <v>0.3739182708900723</v>
       </c>
       <c r="AC24">
-        <v>0.2079502812673658</v>
-      </c>
-      <c r="AD24">
-        <v>0.2357054864565824</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30">
+        <v>0.3328776246135661</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1837,22 +1843,19 @@
         <v>1</v>
       </c>
       <c r="Z25">
-        <v>0.7123884573910364</v>
+        <v>0.7016032992711966</v>
       </c>
       <c r="AA25">
-        <v>0.5252841632244998</v>
+        <v>0.4664725599770774</v>
       </c>
       <c r="AB25">
-        <v>0.3922693189635069</v>
+        <v>0.6342462611946736</v>
       </c>
       <c r="AC25">
-        <v>0.4119602040081735</v>
-      </c>
-      <c r="AD25">
-        <v>0.3564763028322982</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30">
+        <v>0.6962413721077465</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1860,19 +1863,16 @@
         <v>1</v>
       </c>
       <c r="AA26">
-        <v>0.7153767377226827</v>
+        <v>0.8230625388692195</v>
       </c>
       <c r="AB26">
-        <v>0.4759578684568044</v>
+        <v>0.9230504017797204</v>
       </c>
       <c r="AC26">
-        <v>0.6621910310025136</v>
-      </c>
-      <c r="AD26">
-        <v>0.7066349170548821</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30">
+        <v>0.8773409155281611</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1880,16 +1880,13 @@
         <v>1</v>
       </c>
       <c r="AB27">
-        <v>0.8238473963921279</v>
+        <v>0.8288390230457162</v>
       </c>
       <c r="AC27">
-        <v>0.9244694976830347</v>
-      </c>
-      <c r="AD27">
-        <v>0.8813170088844937</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30">
+        <v>0.8329015888832716</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1897,34 +1894,15 @@
         <v>1</v>
       </c>
       <c r="AC28">
-        <v>0.8231175653519607</v>
-      </c>
-      <c r="AD28">
-        <v>0.834460333314026</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30">
+        <v>0.8777715696154577</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AC29">
         <v>1</v>
-      </c>
-      <c r="AD29">
-        <v>0.8791219634797448</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30">
-      <c r="A31" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>